<commit_message>
import testing of incremental HR implementation
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\01_input_data\02_input_prepared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\02_input_prepared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00599DF4-5F71-4A4C-97CB-2F97A27EE279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776B12F7-B4BF-4911-B8B2-2FB851178532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3930" yWindow="-16320" windowWidth="38640" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="180">
   <si>
     <t>Object_Name</t>
   </si>
@@ -1128,7 +1128,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -3995,7 +3997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -4603,8 +4605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5021,6 +5023,9 @@
       <c r="A19" t="s">
         <v>75</v>
       </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
@@ -5032,12 +5037,18 @@
       </c>
       <c r="F19" t="s">
         <v>82</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>75</v>
       </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
@@ -5049,12 +5060,18 @@
       </c>
       <c r="F20" t="s">
         <v>82</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>75</v>
       </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
@@ -5066,6 +5083,9 @@
       </c>
       <c r="F21" t="s">
         <v>82</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-upload of the jupyter document for the new node
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Definition" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Definition_parameters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Definition_parameters_duration" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Nodes" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Connections" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Object__to_from_node_definition" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Object__to_from_node" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Boolean_relations" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Object__node_node" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Variable_Eff" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Time_series_storage" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Demand" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Energy_prices" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Model_components" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Model_relations" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Model" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition_parameters" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition_parameters_duration" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nodes" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connections" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__to_from_node_definition" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__to_from_node" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Boolean_relations" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__node_node" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Variable_Eff" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time_series_storage" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demand" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy_prices" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_components" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_relations" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -523,7 +523,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -535,7 +535,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -547,7 +547,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -583,7 +583,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -595,7 +595,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -607,7 +607,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -619,7 +619,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -631,7 +631,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -643,7 +643,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -655,7 +655,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -667,19 +667,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>node</t>
+          <t>connection</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -703,7 +703,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -715,12 +715,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>Solar_Plant_Kasso_node</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>node</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3360,13 +3360,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3376,11 +3376,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fom_cost</t>
+          <t>unit_on_cost</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.34</v>
+        <v>1e-07</v>
       </c>
     </row>
     <row r="4">
@@ -3396,52 +3396,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fom_cost</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>4.45</v>
+          <t>online_variable_type</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>unit_online_variable_type_integer</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>online_variable_type</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>unit_online_variable_type_integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>power_line_Wholesale_Kasso</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>fom_cost</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D5" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3567,7 +3547,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3577,7 +3557,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -3588,7 +3568,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3598,28 +3578,18 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3635,9 +3605,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3665,7 +3633,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3675,18 +3643,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3707,7 +3677,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3720,9 +3690,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" t="n">
         <v>100000</v>
       </c>
@@ -3730,7 +3708,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3753,7 +3731,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3774,7 +3752,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3797,7 +3775,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3807,18 +3785,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3828,18 +3808,28 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Solar_Plant_Kasso_node</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3847,25 +3837,11 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>100000</v>
-      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4179,19 +4155,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4206,14 +4182,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4223,19 +4199,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4245,12 +4221,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
     </row>
@@ -4272,7 +4248,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
     </row>
@@ -4294,7 +4270,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
     </row>
@@ -4311,19 +4287,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4333,12 +4309,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
@@ -4355,7 +4331,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4367,29 +4343,29 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4404,14 +4380,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4433,7 +4409,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4448,14 +4424,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4465,19 +4441,19 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4492,14 +4468,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4521,7 +4497,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4536,14 +4512,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4553,19 +4529,19 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4580,14 +4556,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4609,7 +4585,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4624,14 +4600,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4641,19 +4617,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4668,29 +4644,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>District_Heating</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Solar_Plant_Kasso_node</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4778,7 +4754,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4788,7 +4764,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -4798,11 +4774,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>ramp_up_limit</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>52</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4">
@@ -4818,21 +4794,21 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>ramp_down_limit</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -4848,21 +4824,21 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>start_up_limit</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>52</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -4878,21 +4854,21 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>shut_down_limit</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>52</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
@@ -4908,27 +4884,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ramp_up_limit</t>
+          <t>minimum_operating_point</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4938,27 +4914,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ramp_down_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4968,21 +4944,21 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>start_up_limit</t>
+          <t>vom_cost</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -4998,27 +4974,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>shut_down_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -5033,16 +5009,22 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>unit_capacity</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -5057,196 +5039,184 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+          <t>Raw_Methanol</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>unit_capacity</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>connection_capacity</t>
+          <t>ramp_up_limit</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>connection_capacity</t>
+          <t>ramp_down_limit</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>connection_capacity</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>1000</v>
-      </c>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>1000</v>
-      </c>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>1000</v>
-      </c>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5256,12 +5226,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -5276,7 +5246,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5286,12 +5256,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -5316,12 +5286,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -5346,20 +5316,200 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>power_line_Wholesale_Kasso</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Power_Wholesale</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>connection__to_node</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>pipeline_storage_hydrogen</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>connection__from_node</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>pipeline_storage_hydrogen</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>connection__to_node</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>pipeline_storage_e-methanol</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>E-Methanol_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>connection__from_node</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>pipeline_storage_e-methanol</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>E-Methanol_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>connection__from_node</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>pipeline_District_Heating</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>connection__to_node</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>pipeline_District_Heating</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
         <is>
           <t>District_Heating</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>connection_capacity</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="F28" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -5457,7 +5607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5534,7 +5684,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.0063</v>
+        <v>4.761428571428572</v>
       </c>
     </row>
     <row r="3">
@@ -5550,17 +5700,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -5569,7 +5719,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>280.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -5585,26 +5735,26 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fix_ratio_in_in_unit_flow</t>
+          <t>fix_ratio_in_out_unit_flow</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>11.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -5620,26 +5770,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>fix_ratio_in_in_unit_flow</t>
+          <t>fix_ratio_in_out_unit_flow</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4.57</v>
+        <v>1.257861635220126</v>
       </c>
     </row>
     <row r="6">
@@ -5655,17 +5805,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -5674,7 +5824,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>1.041666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -5690,26 +5840,26 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fix_ratio_in_out_unit_flow</t>
+          <t>fix_ratio_out_out_unit_flow</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.257861635220126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -5730,91 +5880,91 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fix_ratio_in_out_unit_flow</t>
+          <t>fix_ratio_out_out_unit_flow</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1.041666666666667</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>unit__node__node</t>
+          <t>connection__node__node</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>fix_ratio_out_out_unit_flow</t>
+          <t>fix_ratio_out_in_connection_flow</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1.76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>unit__node__node</t>
+          <t>connection__node__node</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>fix_ratio_out_out_unit_flow</t>
+          <t>fix_ratio_out_in_connection_flow</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>4.32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -5830,17 +5980,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -5865,17 +6015,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -5900,17 +6050,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -5935,17 +6085,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -5960,71 +6110,71 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>connection__node__node</t>
+          <t>unit__node__node</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>fix_ratio_out_in_connection_flow</t>
+          <t>unit_idle_heat_rate</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>connection__node__node</t>
+          <t>unit__node__node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>E-Methanol_Kasso</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>fix_ratio_out_in_connection_flow</t>
+          <t>unit_idle_heat_rate</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17">
@@ -6040,7 +6190,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6050,7 +6200,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -6075,26 +6225,26 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Solar_Plant_Kasso</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>Solar_Plant_Kasso_node</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Power_Kasso</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>unit_idle_heat_rate</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19">
@@ -6110,7 +6260,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6120,16 +6270,16 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>unit_idle_heat_rate</t>
+          <t>unit_incremental_heat_rate</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -6145,7 +6295,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6155,7 +6305,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -6180,7 +6330,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6190,7 +6340,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -6199,41 +6349,6 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>unit__node__node</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Methanol_Reactor</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>unit_incremental_heat_rate</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update methanol input file
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition_parameters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definition_parameters_duration" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nodes" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connections" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__to_from_node_definition" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__to_from_node" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Boolean_relations" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__node_node" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Variable_Eff" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time_series_storage" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demand" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy_prices" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_components" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_relations" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Definition" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Definition_parameters" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Definition_parameters_duration" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Nodes" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Connections" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Object__to_from_node_definition" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Object__to_from_node" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Boolean_relations" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Object__node_node" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Variable_Eff" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Time_series_storage" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Demand" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Energy_prices" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Model_components" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Model_relations" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Model" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -523,7 +523,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -535,7 +535,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -547,7 +547,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -583,7 +583,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -595,7 +595,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -607,7 +607,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -619,7 +619,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -631,7 +631,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -643,7 +643,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -655,7 +655,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -667,19 +667,19 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>node</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -703,7 +703,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -715,12 +715,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso_node</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>node</t>
+          <t>connection</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3360,13 +3360,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3376,11 +3376,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>unit_on_cost</t>
+          <t>fom_cost</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1e-07</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="4">
@@ -3396,32 +3396,52 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>online_variable_type</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>unit_online_variable_type_integer</t>
-        </is>
+          <t>fom_cost</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4.45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Methanol_Reactor</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>online_variable_type</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>unit_online_variable_type_integer</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>connection</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>fom_cost</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>100</v>
       </c>
     </row>
@@ -3547,7 +3567,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3557,7 +3577,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -3568,7 +3588,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3578,18 +3598,28 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3605,7 +3635,9 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3633,7 +3665,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3643,20 +3675,18 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3677,7 +3707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3690,17 +3720,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>100000</v>
       </c>
@@ -3708,7 +3730,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3731,7 +3753,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3752,7 +3774,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3775,7 +3797,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3785,20 +3807,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3808,28 +3828,18 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso_node</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3837,11 +3847,25 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4155,19 +4179,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4182,14 +4206,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4199,19 +4223,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4221,12 +4245,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Steam</t>
         </is>
       </c>
     </row>
@@ -4248,7 +4272,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
@@ -4270,7 +4294,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
     </row>
@@ -4287,19 +4311,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4309,12 +4333,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
     </row>
@@ -4331,7 +4355,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4343,29 +4367,29 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4380,14 +4404,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4409,7 +4433,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4424,14 +4448,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4441,19 +4465,19 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4468,14 +4492,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4497,7 +4521,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4512,14 +4536,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4529,19 +4553,19 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4556,14 +4580,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4585,7 +4609,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4600,14 +4624,14 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4617,19 +4641,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4644,29 +4668,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso_node</t>
+          <t>District_Heating</t>
         </is>
       </c>
     </row>
@@ -4681,7 +4705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4754,7 +4778,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -4764,7 +4788,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -4774,11 +4798,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ramp_up_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -4794,21 +4818,21 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ramp_down_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -4824,21 +4848,21 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>start_up_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -4854,21 +4878,21 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>shut_down_limit</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -4884,27 +4908,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>minimum_operating_point</t>
+          <t>ramp_up_limit</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4914,27 +4938,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>ramp_down_limit</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>52</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>unit__to_node</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4944,21 +4968,21 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>vom_cost</t>
+          <t>start_up_limit</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
@@ -4974,27 +4998,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>shut_down_limit</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -5009,22 +5033,16 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>52</v>
-      </c>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -5039,184 +5057,196 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>100</v>
-      </c>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ramp_up_limit</t>
+          <t>connection_capacity</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ramp_down_limit</t>
+          <t>connection_capacity</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>unit_capacity</t>
+          <t>connection_capacity</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+          <t>Power_Wholesale</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>unit__from_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5226,12 +5256,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -5246,7 +5276,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -5256,12 +5286,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -5286,12 +5316,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -5316,12 +5346,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -5330,186 +5360,6 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>connection__to_node</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>pipeline_storage_hydrogen</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Hydrogen_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>connection__from_node</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>pipeline_storage_hydrogen</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Hydrogen_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>connection__to_node</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>pipeline_storage_e-methanol</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>connection__from_node</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>pipeline_storage_e-methanol</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>connection__from_node</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>pipeline_District_Heating</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>connection__to_node</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>connection</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>pipeline_District_Heating</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>District_Heating</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -5607,7 +5457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5684,7 +5534,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4.761428571428572</v>
+        <v>0.0063</v>
       </c>
     </row>
     <row r="3">
@@ -5700,17 +5550,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -5719,7 +5569,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>280.5</v>
       </c>
     </row>
     <row r="4">
@@ -5735,26 +5585,26 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fix_ratio_in_out_unit_flow</t>
+          <t>fix_ratio_in_in_unit_flow</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="5">
@@ -5770,26 +5620,26 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>fix_ratio_in_out_unit_flow</t>
+          <t>fix_ratio_in_in_unit_flow</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1.257861635220126</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="6">
@@ -5805,17 +5655,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -5824,7 +5674,7 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.041666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -5840,26 +5690,26 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Electrolyzer</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fix_ratio_out_out_unit_flow</t>
+          <t>fix_ratio_in_out_unit_flow</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>1.257861635220126</v>
       </c>
     </row>
     <row r="8">
@@ -5880,91 +5730,91 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Raw_Methanol</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fix_ratio_out_out_unit_flow</t>
+          <t>fix_ratio_in_out_unit_flow</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>1.041666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>connection__node__node</t>
+          <t>unit__node__node</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>fix_ratio_out_in_connection_flow</t>
+          <t>fix_ratio_out_out_unit_flow</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>connection__node__node</t>
+          <t>unit__node__node</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>fix_ratio_out_in_connection_flow</t>
+          <t>fix_ratio_out_out_unit_flow</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="11">
@@ -5980,17 +5830,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -6015,17 +5865,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -6050,17 +5900,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -6085,17 +5935,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -6110,71 +5960,71 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>unit__node__node</t>
+          <t>connection__node__node</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>unit_idle_heat_rate</t>
+          <t>fix_ratio_out_in_connection_flow</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>unit__node__node</t>
+          <t>connection__node__node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>unit_idle_heat_rate</t>
+          <t>fix_ratio_out_in_connection_flow</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -6190,7 +6040,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6200,7 +6050,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -6225,17 +6075,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Solar_Plant_Kasso_node</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -6244,7 +6094,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
@@ -6260,7 +6110,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6270,16 +6120,16 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>unit_incremental_heat_rate</t>
+          <t>unit_idle_heat_rate</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
@@ -6295,7 +6145,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6305,7 +6155,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -6330,25 +6180,60 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Destilation_Tower</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>unit_incremental_heat_rate</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>unit__node__node</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Methanol_Reactor</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Power_Kasso</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>Raw_Methanol</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>unit_incremental_heat_rate</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="G22" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update mapping to new op input
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -17,12 +17,13 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Boolean_relations" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object__node_node" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Variable_Eff" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time_series_storage" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demand" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy_prices" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_components" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_relations" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Operating_points" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time_series_storage" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demand" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Energy_prices" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_components" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model_relations" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -535,7 +536,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -547,7 +548,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -559,7 +560,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -571,7 +572,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -583,7 +584,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -595,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -607,7 +608,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -619,7 +620,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -631,7 +632,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -643,7 +644,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -655,7 +656,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -667,7 +668,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -679,7 +680,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -985,6 +986,161 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>relationship_class:</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>unit__from_node</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Electrolyzer</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>node</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>node</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>parameter name</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>operating_points</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1050,7 +1206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1895,7 +2051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2792,7 +2948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2943,7 +3099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3286,7 +3442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3680,7 +3836,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3703,7 +3859,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3713,20 +3869,18 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3736,20 +3890,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3772,7 +3924,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3782,20 +3934,18 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3805,18 +3955,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3826,18 +3978,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3847,18 +4001,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3871,9 +4027,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" t="n">
         <v>100000</v>
       </c>
@@ -3881,7 +4045,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3894,9 +4058,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" t="n">
         <v>100000</v>
       </c>
@@ -3904,7 +4076,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3914,28 +4086,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3945,18 +4107,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3969,17 +4133,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>100000</v>
       </c>

</xml_diff>

<commit_message>
fix operating points bug in data prep
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -548,7 +548,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -572,7 +572,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -620,7 +620,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -644,7 +644,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.1307738452309538</v>
       </c>
     </row>
     <row r="7">
@@ -1063,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.2273545290941812</v>
       </c>
     </row>
     <row r="8">
@@ -1071,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>0.3239352129574085</v>
       </c>
     </row>
     <row r="9">
@@ -1079,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>0.4205158968206358</v>
       </c>
     </row>
     <row r="10">
@@ -1087,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>0.5170965806838632</v>
       </c>
     </row>
     <row r="11">
@@ -1095,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>0.6136772645470906</v>
       </c>
     </row>
     <row r="12">
@@ -1103,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>0.710257948410318</v>
       </c>
     </row>
     <row r="13">
@@ -1111,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>0.8068386322735454</v>
       </c>
     </row>
     <row r="14">
@@ -1119,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>0.9034193161367727</v>
       </c>
     </row>
     <row r="15">
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3448,7 +3448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3561,33 +3561,6 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>{"type":"duration", "data": "1h"}</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>toy</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>roll_forward</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Base</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>{"type": "duration", "data": "4h"}</t>
         </is>
       </c>
     </row>
@@ -3859,7 +3832,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3880,7 +3853,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3890,18 +3863,28 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3924,7 +3907,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3945,7 +3928,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3968,7 +3951,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3978,20 +3961,18 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4001,15 +3982,13 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4045,7 +4024,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4058,17 +4037,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>100000</v>
       </c>
@@ -4076,7 +4047,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4086,18 +4057,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">

</xml_diff>

<commit_message>
data prep test run
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -536,7 +536,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -572,7 +572,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -620,7 +620,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -632,7 +632,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -644,7 +644,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -680,7 +680,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3809,7 +3809,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3842,18 +3842,28 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3863,28 +3873,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3907,7 +3907,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3917,18 +3917,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3941,9 +3943,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" t="n">
         <v>100000</v>
       </c>
@@ -3951,7 +3961,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3961,18 +3971,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3993,7 +4005,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4003,28 +4015,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4047,7 +4049,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4057,20 +4059,18 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4093,7 +4093,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">

</xml_diff>

<commit_message>
remove old input links
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_Input_prepared.xlsx
@@ -536,7 +536,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -572,7 +572,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -596,7 +596,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -620,7 +620,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -632,7 +632,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -644,7 +644,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -680,7 +680,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3809,7 +3809,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3819,18 +3819,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3853,7 +3855,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3863,28 +3865,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3894,20 +3886,18 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3928,7 +3918,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3941,17 +3931,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>100000</v>
       </c>
@@ -3959,7 +3941,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3982,7 +3964,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4005,7 +3987,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4015,20 +3997,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4041,9 +4021,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" t="n">
         <v>100000</v>
       </c>
@@ -4051,7 +4039,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4061,18 +4049,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4082,18 +4072,28 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">

</xml_diff>